<commit_message>
Add color column to sample data
</commit_message>
<xml_diff>
--- a/data/sampleDDS.xlsx
+++ b/data/sampleDDS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cw/Documents/rCode/disasterDeclarations/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cw/Documents/rCode/femaDisasterDeclarations/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20071291-7E9B-D348-BDD7-20EBCFED3D88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA4D92ED-8860-8442-86B9-887DCB919884}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16540" xr2:uid="{86D19621-03E1-484D-97BF-605221549BB9}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
   <si>
     <t>state</t>
   </si>
@@ -135,6 +135,27 @@
   </si>
   <si>
     <t>long</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>orange</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>brown</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>yellow</t>
   </si>
 </sst>
 </file>
@@ -486,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78551E3D-7E45-3F4C-95C8-C3649C1FBD5B}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="118" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -501,7 +522,7 @@
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -523,8 +544,11 @@
       <c r="G1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -546,8 +570,11 @@
       <c r="G2">
         <v>-101.44240000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -569,8 +596,11 @@
       <c r="G3">
         <v>-93.338899999999995</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -592,8 +622,11 @@
       <c r="G4">
         <v>-85.147900000000007</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -615,8 +648,11 @@
       <c r="G5">
         <v>-77.436000000000007</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -638,8 +674,11 @@
       <c r="G6">
         <v>-81.559600000000003</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -661,8 +700,11 @@
       <c r="G7">
         <v>-92.539599999999993</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -684,8 +726,11 @@
       <c r="G8">
         <v>-98.221299999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -706,6 +751,9 @@
       </c>
       <c r="G9">
         <v>-96.835099999999997</v>
+      </c>
+      <c r="H9" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>